<commit_message>
Update Nets.eli, Nets_cleaned.eli, and 7 more files...
</commit_message>
<xml_diff>
--- a/status.xlsx
+++ b/status.xlsx
@@ -451,7 +451,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +546,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" t="s">
@@ -554,7 +554,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
@@ -570,7 +570,7 @@
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>